<commit_message>
Adaugare de cerinte noi in Cerinte.xlsx
</commit_message>
<xml_diff>
--- a/Cerinte.xlsx
+++ b/Cerinte.xlsx
@@ -24,23 +24,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Adaugare Articol Roata</t>
   </si>
   <si>
-    <t>Stergere Articol Roata</t>
-  </si>
-  <si>
     <t>Modificare Articol Roata</t>
   </si>
   <si>
     <t>Afisarea tuturor articolelor</t>
   </si>
   <si>
-    <t>Afisarea articolelor in baza unui filtru dupa : (toate campurile articolului roata)</t>
-  </si>
-  <si>
     <t>Afisarea sub forma de statistica a sumelor articolelor . Toate articolele vandute pe o anumita perioada, toate articolele vandute pe o anumita peropada pe categori(dupa firma, sau alte criterii)</t>
   </si>
   <si>
@@ -48,6 +42,57 @@
   </si>
   <si>
     <t>Comentariu</t>
+  </si>
+  <si>
+    <t>Responsabil de implementare</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>deocamdata doar rotile</t>
+  </si>
+  <si>
+    <t>Salvarea datelor intr-o baza de date pe Claud</t>
+  </si>
+  <si>
+    <t>introducere functionalitate scanner QR (2D)</t>
+  </si>
+  <si>
+    <t>Afisare articol(roata) pe o singura pagina (full description)</t>
+  </si>
+  <si>
+    <t>Logare cu user si parola, logarea sa se faca doar o data pe zi (userul si parola se salveaza pe device sub forma the hash) . In baza de date se salveaza user, parola, si hash-ul.</t>
+  </si>
+  <si>
+    <t>Prioritate</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>in lucru</t>
+  </si>
+  <si>
+    <t>terminat</t>
+  </si>
+  <si>
+    <t>Afisarea articolelor in baza unui filtru dupa : (toate campurile articolului roata), Serial Number (SN)</t>
+  </si>
+  <si>
+    <t>Stergere Articol Roata (se face prin update al campului disponibil cu false)</t>
+  </si>
+  <si>
+    <t>Cautare Articol Scanat</t>
+  </si>
+  <si>
+    <t>Filtrare dupa articolul Scanat</t>
+  </si>
+  <si>
+    <t>Drepturi user pe tipuri de utilizatori (admin, worker, vizitator)</t>
+  </si>
+  <si>
+    <t>Readucere Articol ca disponibil</t>
   </si>
 </sst>
 </file>
@@ -78,7 +123,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -201,42 +246,123 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -249,7 +375,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -258,19 +384,62 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -585,211 +754,334 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D26"/>
+  <dimension ref="B1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="4.5546875" customWidth="1"/>
-    <col min="3" max="3" width="57.88671875" customWidth="1"/>
-    <col min="4" max="4" width="15.21875" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="57.88671875" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="17" style="22" customWidth="1"/>
+    <col min="7" max="7" width="15.21875" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="10"/>
-      <c r="C2" s="11" t="s">
+    <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="20"/>
+      <c r="C2" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="F2" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="5">
+        <v>1</v>
+      </c>
+      <c r="C3" s="17">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="7">
-        <v>1</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="9"/>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="14"/>
+    </row>
+    <row r="4" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B4" s="3">
         <f>B3+1</f>
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="18">
         <v>1</v>
       </c>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="15"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="3">
-        <f t="shared" ref="B5:B22" si="0">B4+1</f>
+        <f t="shared" ref="B5:B21" si="0">B4+1</f>
         <v>3</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="18">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="15"/>
+    </row>
+    <row r="6" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B6" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C6" s="18">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="3">
-        <f t="shared" si="0"/>
+      <c r="E6" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B7" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C7" s="18">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="15"/>
+    </row>
+    <row r="8" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B8" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C8" s="18">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="15"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="3">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C9" s="18">
+        <v>3</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="15"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C10" s="18">
+        <v>3</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="15"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="3">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C11" s="18">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="15"/>
+    </row>
+    <row r="12" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B12" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C12" s="18">
+        <v>3</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="15"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="3">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C13" s="18">
         <v>4</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B7" s="3">
-        <f t="shared" si="0"/>
+      <c r="D13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="15"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="3">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C14" s="18">
+        <v>4</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="15"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="3">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="C15" s="18">
         <v>5</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B8" s="3">
-        <f t="shared" si="0"/>
+      <c r="D15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="15"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B16" s="3">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="C16" s="18">
         <v>6</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="3">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B10" s="3">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B11" s="3">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B12" s="3">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B13" s="3">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B14" s="3">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B15" s="3">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B16" s="3">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="15"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C17" s="18"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="15"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C18" s="18"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="15"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C19" s="18"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="15"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C20" s="18"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="15"/>
+    </row>
+    <row r="21" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C21" s="2"/>
+      <c r="C21" s="19"/>
       <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="3">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="6"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C26" s="1"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="16"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="25"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="25"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="25"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changed status in Cerinte.xlsx
</commit_message>
<xml_diff>
--- a/Cerinte.xlsx
+++ b/Cerinte.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>Adaugare Articol Roata</t>
   </si>
@@ -756,8 +756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -929,8 +929,12 @@
       <c r="D11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
+      <c r="E11" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>15</v>
+      </c>
       <c r="G11" s="15"/>
     </row>
     <row r="12" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">

</xml_diff>